<commit_message>
refactor(Proveedores - Solicitud): Agregadas horas de inicio y finalización
</commit_message>
<xml_diff>
--- a/archivos/plantillas/proveedores_importacion_solicitud_cotizacion.xlsx
+++ b/archivos/plantillas/proveedores_importacion_solicitud_cotizacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Proyectos\Simón Bolívar\Módulo de proveedores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectos\simon-bolivar\archivos\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A5A7CB-B14D-4043-B36D-8CC36D6E2D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57155495-286C-4D3B-834D-A9A793DAE8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8ADAB593-72DA-4AED-8D36-AA0FAA89A16B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8ADAB593-72DA-4AED-8D36-AA0FAA89A16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Fecha de inicio</t>
   </si>
@@ -48,12 +48,15 @@
   <si>
     <t>Cantidad</t>
   </si>
+  <si>
+    <t>Hora</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +75,28 @@
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF19287F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,15 +104,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color theme="0"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color theme="0"/>
+      </right>
+      <top style="hair">
+        <color theme="0"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -106,6 +144,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,57 +471,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5ED38-F96E-4CC7-A802-43EAA271DABC}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="13.5703125" style="3"/>
+    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="13.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <v>45835</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2">
-        <v>45835</v>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>4917</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>15602</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>